<commit_message>
etage 2 modifier compaire high card
</commit_message>
<xml_diff>
--- a/DefinitionEtSuiviDeTaches-v02.xlsx
+++ b/DefinitionEtSuiviDeTaches-v02.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\JAVA Project\poker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Définition</t>
   </si>
@@ -166,53 +158,46 @@
   </si>
   <si>
     <t>Avancement des releases</t>
-  </si>
-  <si>
-    <t>Oui</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="DengXian"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="DengXian"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="DengXian"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color indexed="16"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -236,12 +221,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -314,69 +301,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="差" xfId="1" builtinId="27"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="适中" xfId="2" builtinId="28"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="ff006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -387,18 +406,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="10"/>
-          <bgColor indexed="15"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
+        <color rgb="ff006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -417,7 +425,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="ff006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -428,7 +436,18 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="ff9c5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="10"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -441,85 +460,32 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFD8D8D8"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffd8d8d8"/>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="FFC6EFCE"/>
-      <rgbColor rgb="FF006100"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFFC7CE"/>
-      <rgbColor rgb="FFFFEB9C"/>
-      <rgbColor rgb="FF9C5700"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ffc6efce"/>
+      <rgbColor rgb="ff006100"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffffc7ce"/>
+      <rgbColor rgb="ffffeb9c"/>
+      <rgbColor rgb="ff9c5700"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff9c0006"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Thème Office">
       <a:dk1>
@@ -711,17 +677,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -740,19 +706,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -770,7 +736,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -796,7 +762,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -822,7 +788,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -848,7 +814,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -874,7 +840,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -900,7 +866,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -926,7 +892,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -952,7 +918,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -978,7 +944,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,32 +957,26 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1035,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1061,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1087,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1113,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1139,7 +1099,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1165,7 +1125,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1191,7 +1151,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1217,7 +1177,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1243,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1269,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1282,15 +1242,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1304,7 +1258,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1323,19 +1277,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1353,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1379,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1405,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1431,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1457,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1483,7 +1437,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1509,7 +1463,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1535,7 +1489,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1561,7 +1515,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1574,449 +1528,450 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV15"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6719" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="256" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" customWidth="1"/>
+    <col min="11" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" ht="17.1" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="17.1" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" ht="45" customHeight="1">
+      <c r="A3" s="6">
         <f>ROW(A3)-2</f>
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>49</v>
+      <c r="H3" s="6">
+        <v>16.02</v>
+      </c>
+      <c r="I3" s="6">
+        <v>18.02</v>
+      </c>
+      <c r="J3" t="s" s="4">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" customHeight="1">
-      <c r="A4" s="4">
+    <row r="4" ht="45" customHeight="1">
+      <c r="A4" s="6">
         <f>ROW(A4)-2</f>
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="H4" s="6">
+        <v>18.02</v>
+      </c>
+      <c r="I4" s="6">
+        <v>20.02</v>
+      </c>
+      <c r="J4" t="s" s="4">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="45" customHeight="1">
-      <c r="A5" s="4">
+    <row r="5" ht="45" customHeight="1">
+      <c r="A5" s="6">
         <f>ROW(A5)-2</f>
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s" s="4">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="H5" s="6">
+        <v>20.02</v>
+      </c>
+      <c r="I5" s="6">
+        <v>22.02</v>
+      </c>
+      <c r="J5" t="s" s="4">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="45" customHeight="1">
-      <c r="A6" s="4">
+    <row r="6" ht="45" customHeight="1">
+      <c r="A6" s="6">
         <f>ROW(A6)-2</f>
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="45" customHeight="1">
-      <c r="A7" s="4">
+    <row r="7" ht="45" customHeight="1">
+      <c r="A7" s="6">
         <f>ROW(A7)-2</f>
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="45" customHeight="1">
-      <c r="A8" s="6">
+    <row r="8" ht="45" customHeight="1">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" t="s" s="11">
         <v>15</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" t="s" s="11">
         <v>34</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" t="s" s="12">
         <v>29</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" ht="45" customHeight="1">
-      <c r="A9" s="11">
+    <row r="9" ht="45" customHeight="1">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" t="s" s="16">
         <v>30</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" t="s" s="17">
         <v>20</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" t="s" s="17">
         <v>15</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" t="s" s="18">
         <v>37</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="45" customHeight="1">
-      <c r="A10" s="15">
+    <row r="10" ht="45" customHeight="1">
+      <c r="A10" s="20">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" t="s" s="21">
         <v>38</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" t="s" s="21">
         <v>39</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" t="s" s="22">
         <v>24</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" t="s" s="22">
         <v>15</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" t="s" s="22">
         <v>40</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" t="s" s="23">
         <v>37</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="1:10" ht="45" customHeight="1">
-      <c r="A11" s="15">
+    <row r="11" ht="45" customHeight="1">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" t="s" s="21">
         <v>38</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" t="s" s="21">
         <v>41</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" t="s" s="22">
         <v>14</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" t="s" s="22">
         <v>15</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" t="s" s="23">
         <v>37</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
     </row>
-    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="15">
+    <row r="12" ht="17.1" customHeight="1">
+      <c r="A12" s="20">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" t="s" s="21">
         <v>43</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" t="s" s="21">
         <v>44</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" t="s" s="22">
         <v>45</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" t="s" s="22">
         <v>15</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" t="s" s="22">
         <v>46</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" t="s" s="22">
         <v>47</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="18" t="s">
+    <row r="13" ht="17.1" customHeight="1">
+      <c r="A13" t="s" s="24">
         <v>48</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
-    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="20">
+    <row r="14" ht="17.1" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="26">
         <v>1</v>
       </c>
-      <c r="C14" s="19" t="e">
+      <c r="C14" s="25">
         <f>COUNTIFS($F$3:$F$7,B14,$J$3:$J$7,"=OK")/COUNTIF($F$3:$F$7,B14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
     </row>
-    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="20">
+    <row r="15" ht="17.1" customHeight="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="26">
         <f>B14+1</f>
         <v>2</v>
       </c>
-      <c r="C15" s="19" t="e">
+      <c r="C15" s="25">
         <f>COUNTIFS($F$3:$F$7,B15,$J$3:$J$7,"=OK")/COUNTIF($F$3:$F$7,B15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A1:G3 A4:F15 G12:G15">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J2 H3:I7 I8:J15">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal" stopIfTrue="1">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J7">
-    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" text="NOK">
       <formula>NOT(ISERROR(FIND(UPPER("NOK"),UPPER(J3))))</formula>
       <formula>"NOK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal" stopIfTrue="1">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G11">
-    <cfRule type="containsText" dxfId="1" priority="4" stopIfTrue="1" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" text="PF">
       <formula>NOT(ISERROR(FIND(UPPER("PF"),UPPER(G4))))</formula>
       <formula>"PF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal" stopIfTrue="1">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
fix bug to the final goal
</commit_message>
<xml_diff>
--- a/DefinitionEtSuiviDeTaches-v02.xlsx
+++ b/DefinitionEtSuiviDeTaches-v02.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>Définition</t>
   </si>
@@ -241,6 +241,10 @@
   </si>
   <si>
     <t>Version 3.0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oui</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1662,7 +1666,7 @@
   <dimension ref="A1:IV17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -2106,9 +2110,15 @@
       <c r="G14" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="H14" s="17">
+        <v>4.03</v>
+      </c>
+      <c r="I14" s="17">
+        <v>4.03</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="22" t="s">

</xml_diff>